<commit_message>
locator helper and keywords
</commit_message>
<xml_diff>
--- a/resources/keywords.xlsx
+++ b/resources/keywords.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="testcases" sheetId="1" r:id="rId1"/>
+    <sheet name="teststeps" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,55 +20,209 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>heading</t>
-  </si>
-  <si>
-    <t>data1</t>
-  </si>
-  <si>
-    <t>data2</t>
-  </si>
-  <si>
-    <t>data3</t>
-  </si>
-  <si>
-    <t>data4</t>
-  </si>
-  <si>
-    <t>data5</t>
-  </si>
-  <si>
-    <t>heading2</t>
-  </si>
-  <si>
-    <t>data12</t>
-  </si>
-  <si>
-    <t>data22</t>
-  </si>
-  <si>
-    <t>data32</t>
-  </si>
-  <si>
-    <t>data42</t>
-  </si>
-  <si>
-    <t>data52</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
+  <si>
+    <t>Test case ID</t>
+  </si>
+  <si>
+    <t>Test Case Name</t>
+  </si>
+  <si>
+    <t>Run Mode</t>
+  </si>
+  <si>
+    <t>TC_Login_001</t>
+  </si>
+  <si>
+    <t>TC_EditInfo_002</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>edit general info</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Test step name</t>
+  </si>
+  <si>
+    <t>Loc Type</t>
+  </si>
+  <si>
+    <t>Loc Value</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>open browser</t>
+  </si>
+  <si>
+    <t>openBrowser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>navigate to url</t>
+  </si>
+  <si>
+    <t>http://apps.qaplanet.in/qahrm/login.php</t>
+  </si>
+  <si>
+    <t>navigate</t>
+  </si>
+  <si>
+    <t>enter user name with valid data</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>txtUserName</t>
+  </si>
+  <si>
+    <t>setText</t>
+  </si>
+  <si>
+    <t>qaplanet1</t>
+  </si>
+  <si>
+    <t>enter password with valid data</t>
+  </si>
+  <si>
+    <t>txtPassword</t>
+  </si>
+  <si>
+    <t>lab1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">click on login button </t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>move to admin</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>//li[@id='admin']/a</t>
+  </si>
+  <si>
+    <t>moveToElement</t>
+  </si>
+  <si>
+    <t>move to company info</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Company Info')]</t>
+  </si>
+  <si>
+    <t>move to General and click</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'General')]</t>
+  </si>
+  <si>
+    <t>moveToEleAndClick</t>
+  </si>
+  <si>
+    <t>switch to frame</t>
+  </si>
+  <si>
+    <t>//iframe[@id='rightMenu']</t>
+  </si>
+  <si>
+    <t>switchToFrame</t>
+  </si>
+  <si>
+    <t>click on edit button</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>editBtn</t>
+  </si>
+  <si>
+    <t>change city name</t>
+  </si>
+  <si>
+    <t>cmbCity</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>select country</t>
+  </si>
+  <si>
+    <t>cmbCountry</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>click on save button</t>
+  </si>
+  <si>
+    <t>switch to default content</t>
+  </si>
+  <si>
+    <t>switchToDefaultContent</t>
+  </si>
+  <si>
+    <t>click on logout button</t>
+  </si>
+  <si>
+    <t>//a[text()='Logout']</t>
+  </si>
+  <si>
+    <t>close the browser</t>
+  </si>
+  <si>
+    <t>closeBrowser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,8 +245,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,63 +545,494 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
driver class which runs everything
</commit_message>
<xml_diff>
--- a/resources/keywords.xlsx
+++ b/resources/keywords.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="testcases" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
     <t>TC_Login_001</t>
   </si>
   <si>
-    <t>TC_EditInfo_002</t>
-  </si>
-  <si>
     <t>login</t>
   </si>
   <si>
@@ -197,6 +194,9 @@
   </si>
   <si>
     <t>closeBrowser</t>
+  </si>
+  <si>
+    <t>TC_Editinfo_002</t>
   </si>
 </sst>
 </file>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,21 +574,21 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -599,10 +599,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -620,416 +620,304 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="E8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>44</v>
-      </c>
       <c r="E11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="E14" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="E16" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>